<commit_message>
ACTUALIZACIONES al 13 11
</commit_message>
<xml_diff>
--- a/Resultado Analisis Microsoft Entre de Consein.xlsx
+++ b/Resultado Analisis Microsoft Entre de Consein.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conseincloud-my.sharepoint.com/personal/wrivas_consein_com/Documents/Documents/Proyectos VSCODE/entraid-bench/entraid-bench/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF1B53CE-932F-47BA-931F-3078889862E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{EF1B53CE-932F-47BA-931F-3078889862E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC54FA87-12F8-431A-AACB-B4A5931589A1}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{609879FC-E90F-4D25-8BF3-ABF7DD2CC9EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{609879FC-E90F-4D25-8BF3-ABF7DD2CC9EB}"/>
   </bookViews>
   <sheets>
     <sheet name="scan_results" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">scan_results!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -953,9 +954,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1406,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689C65CF-690C-4AC0-8D64-C4D0513E5A7F}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1451,551 +1451,551 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>69</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2011,7 +2011,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B27912-D836-406A-B193-AF60728C0981}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:G118"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2048,2693 +2050,2693 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>112</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>113</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>118</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>121</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>124</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>126</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>128</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>129</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>130</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>136</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>137</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>141</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>136</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>137</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>137</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
         <v>144</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>137</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>137</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>137</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
         <v>147</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>150</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>137</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>137</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>151</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>152</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>153</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>155</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>153</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
         <v>156</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>157</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>153</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="s">
         <v>158</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>159</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>152</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>153</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="1" t="s">
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>161</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>152</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>153</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="1" t="s">
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
         <v>162</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>163</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>164</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>165</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="1" t="s">
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
         <v>166</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>167</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>168</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
         <v>169</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>167</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>168</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
         <v>170</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>167</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>168</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
         <v>171</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>167</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>168</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
         <v>172</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>167</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>168</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
         <v>173</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>167</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>168</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
         <v>174</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>168</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>175</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>176</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>177</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>178</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>179</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>180</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>181</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
         <v>162</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>163</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>183</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>184</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>108</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>183</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>184</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="1" t="s">
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
         <v>147</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>148</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>185</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>186</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="1" t="s">
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
         <v>187</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>188</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>189</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>190</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="1" t="s">
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
         <v>191</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>192</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>193</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>194</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="1" t="s">
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" t="s">
         <v>191</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>192</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>195</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="1" t="s">
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
         <v>197</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>198</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>195</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>196</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="A50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" t="s">
         <v>197</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>198</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>199</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>200</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="1" t="s">
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="A51" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" t="s">
         <v>197</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>198</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>201</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>202</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="1" t="s">
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="A52" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" t="s">
         <v>197</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>198</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>203</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>204</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="1" t="s">
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="A53" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" t="s">
         <v>197</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>198</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>205</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>206</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="1" t="s">
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="A54" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" t="s">
         <v>197</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>198</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>207</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>208</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="1" t="s">
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="A55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>209</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>210</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="1" t="s">
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="A56" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" t="s">
         <v>197</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>198</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>209</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>210</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="1" t="s">
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="A57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>98</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>211</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>212</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="1" t="s">
+      <c r="F57" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="A58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" t="s">
         <v>191</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>192</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>211</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>212</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="1" t="s">
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="A59" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" t="s">
         <v>213</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>214</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>215</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>216</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="1" t="s">
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="A60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" t="s">
         <v>217</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>218</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>219</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>220</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="1" t="s">
+      <c r="F60" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="A61" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" t="s">
         <v>221</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>222</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>219</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>220</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="1" t="s">
+      <c r="F61" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" t="s">
         <v>223</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>224</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" t="s">
         <v>225</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>226</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="1" t="s">
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" t="s">
         <v>227</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>228</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" t="s">
         <v>225</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>226</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="1" t="s">
+      <c r="F63" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" t="s">
         <v>229</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>230</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>231</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>232</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="1" t="s">
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="A65" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" t="s">
         <v>229</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>233</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>231</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>232</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="F65" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="A66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" t="s">
         <v>229</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>234</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>231</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>232</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="1" t="s">
+      <c r="F66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B67" s="1" t="s">
+      <c r="A67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" t="s">
         <v>229</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>235</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>231</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>232</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="1" t="s">
+      <c r="F67" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B68" s="1" t="s">
+      <c r="A68" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
         <v>162</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>163</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>110</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>111</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="1" t="s">
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B69" s="1" t="s">
+      <c r="A69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" t="s">
         <v>145</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>146</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>236</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>237</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="1" t="s">
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="A70" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" t="s">
         <v>107</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>108</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" t="s">
         <v>236</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>237</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="1" t="s">
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B71" s="1" t="s">
+      <c r="A71" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" t="s">
         <v>146</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>238</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>239</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="1" t="s">
+      <c r="F71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="A72" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" t="s">
         <v>162</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>163</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>240</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>241</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G72" s="1" t="s">
+      <c r="F72" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B73" s="1" t="s">
+      <c r="A73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>93</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>242</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" t="s">
         <v>243</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="1" t="s">
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B74" s="1" t="s">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" t="s">
         <v>187</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>188</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>242</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" t="s">
         <v>243</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" s="1" t="s">
+      <c r="F74" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B75" s="1" t="s">
+      <c r="A75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" t="s">
         <v>191</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>192</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>242</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" t="s">
         <v>243</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="1" t="s">
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B76" s="1" t="s">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" t="s">
         <v>223</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>224</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>242</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>243</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G76" s="1" t="s">
+      <c r="F76" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B77" s="1" t="s">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" t="s">
         <v>244</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" t="s">
         <v>245</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" t="s">
         <v>246</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>247</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" s="1" t="s">
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B78" s="1" t="s">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" t="s">
         <v>97</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" t="s">
         <v>98</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" t="s">
         <v>248</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" t="s">
         <v>249</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" s="1" t="s">
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B79" s="1" t="s">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" t="s">
         <v>97</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>98</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" t="s">
         <v>250</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" t="s">
         <v>251</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="1" t="s">
+      <c r="F79" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B80" s="1" t="s">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" t="s">
         <v>217</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" t="s">
         <v>218</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" t="s">
         <v>252</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" t="s">
         <v>253</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G80" s="1" t="s">
+      <c r="F80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" s="1" t="s">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" t="s">
         <v>254</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" t="s">
         <v>255</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" t="s">
         <v>252</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" t="s">
         <v>253</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" s="1" t="s">
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B82" s="1" t="s">
+      <c r="A82" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" t="s">
         <v>145</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" t="s">
         <v>151</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" t="s">
         <v>252</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" t="s">
         <v>253</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G82" s="1" t="s">
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B83" s="1" t="s">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" t="s">
         <v>256</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" t="s">
         <v>257</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" t="s">
         <v>252</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" t="s">
         <v>253</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" s="1" t="s">
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B84" s="1" t="s">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" t="s">
         <v>156</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" t="s">
         <v>252</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" t="s">
         <v>253</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G84" s="1" t="s">
+      <c r="F84" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B85" s="1" t="s">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" t="s">
         <v>254</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" t="s">
         <v>255</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" t="s">
         <v>258</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" t="s">
         <v>259</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G85" s="1" t="s">
+      <c r="F85" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B86" s="1" t="s">
+      <c r="A86" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" t="s">
         <v>254</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>255</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" t="s">
         <v>260</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E86" t="s">
         <v>261</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G86" s="1" t="s">
+      <c r="F86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" s="1" t="s">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" t="s">
         <v>254</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>255</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" t="s">
         <v>262</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E87" t="s">
         <v>263</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G87" s="1" t="s">
+      <c r="F87" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B88" s="1" t="s">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" t="s">
         <v>264</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" t="s">
         <v>265</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" t="s">
         <v>104</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>105</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G88" s="1" t="s">
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B89" s="1" t="s">
+      <c r="A89" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" t="s">
         <v>147</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" t="s">
         <v>148</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" t="s">
         <v>104</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" t="s">
         <v>105</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="1" t="s">
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B90" s="1" t="s">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
         <v>191</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" t="s">
         <v>192</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" t="s">
         <v>104</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>105</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" s="1" t="s">
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" s="1" t="s">
+      <c r="A91" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
         <v>221</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" t="s">
         <v>222</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" t="s">
         <v>94</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" t="s">
         <v>95</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G91" s="1" t="s">
+      <c r="F91" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B92" s="1" t="s">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
         <v>266</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" t="s">
         <v>267</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" t="s">
         <v>94</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" t="s">
         <v>95</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G92" s="1" t="s">
+      <c r="F92" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" s="1" t="s">
+      <c r="A93" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
         <v>187</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" t="s">
         <v>188</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" t="s">
         <v>94</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" t="s">
         <v>95</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G93" s="1" t="s">
+      <c r="F93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B94" s="1" t="s">
+      <c r="A94" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" t="s">
         <v>268</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" t="s">
         <v>269</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" t="s">
         <v>94</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E94" t="s">
         <v>95</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G94" s="1" t="s">
+      <c r="F94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B95" s="1" t="s">
+      <c r="A95" t="s">
+        <v>91</v>
+      </c>
+      <c r="B95" t="s">
         <v>270</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" t="s">
         <v>271</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E95" t="s">
         <v>95</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G95" s="1" t="s">
+      <c r="F95" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B96" s="1" t="s">
+      <c r="A96" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" t="s">
         <v>191</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" t="s">
         <v>192</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" t="s">
         <v>94</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E96" t="s">
         <v>95</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G96" s="1" t="s">
+      <c r="F96" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B97" s="1" t="s">
+      <c r="A97" t="s">
+        <v>91</v>
+      </c>
+      <c r="B97" t="s">
         <v>197</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" t="s">
         <v>198</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" t="s">
         <v>94</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E97" t="s">
         <v>95</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G97" s="1" t="s">
+      <c r="F97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B98" s="1" t="s">
+      <c r="A98" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" t="s">
         <v>223</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" t="s">
         <v>94</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E98" t="s">
         <v>95</v>
       </c>
-      <c r="F98" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G98" s="1" t="s">
+      <c r="F98" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B99" s="1" t="s">
+      <c r="A99" t="s">
+        <v>91</v>
+      </c>
+      <c r="B99" t="s">
         <v>187</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" t="s">
         <v>188</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" t="s">
         <v>272</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E99" t="s">
         <v>273</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G99" s="1" t="s">
+      <c r="F99" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B100" s="1" t="s">
+      <c r="A100" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" t="s">
         <v>98</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" t="s">
         <v>272</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E100" t="s">
         <v>273</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G100" s="1" t="s">
+      <c r="F100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B101" s="1" t="s">
+      <c r="A101" t="s">
+        <v>91</v>
+      </c>
+      <c r="B101" t="s">
         <v>191</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" t="s">
         <v>192</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" t="s">
         <v>272</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" t="s">
         <v>273</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G101" s="1" t="s">
+      <c r="F101" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B102" s="1" t="s">
+      <c r="A102" t="s">
+        <v>91</v>
+      </c>
+      <c r="B102" t="s">
         <v>223</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" t="s">
         <v>224</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" t="s">
         <v>272</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E102" t="s">
         <v>273</v>
       </c>
-      <c r="F102" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G102" s="1" t="s">
+      <c r="F102" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B103" s="1" t="s">
+      <c r="A103" t="s">
+        <v>91</v>
+      </c>
+      <c r="B103" t="s">
         <v>162</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" t="s">
         <v>163</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" t="s">
         <v>274</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E103" t="s">
         <v>275</v>
       </c>
-      <c r="F103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G103" s="1" t="s">
+      <c r="F103" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B104" s="1" t="s">
+      <c r="A104" t="s">
+        <v>91</v>
+      </c>
+      <c r="B104" t="s">
         <v>276</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" t="s">
         <v>277</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" t="s">
         <v>274</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E104" t="s">
         <v>275</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G104" s="1" t="s">
+      <c r="F104" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B105" s="1" t="s">
+      <c r="A105" t="s">
+        <v>91</v>
+      </c>
+      <c r="B105" t="s">
         <v>278</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" t="s">
         <v>279</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" t="s">
         <v>274</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="E105" t="s">
         <v>275</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" s="1" t="s">
+      <c r="F105" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B106" s="1" t="s">
+      <c r="A106" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106" t="s">
         <v>197</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" t="s">
         <v>198</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" t="s">
         <v>274</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E106" t="s">
         <v>275</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G106" s="1" t="s">
+      <c r="F106" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B107" s="1" t="s">
+      <c r="A107" t="s">
+        <v>91</v>
+      </c>
+      <c r="B107" t="s">
         <v>92</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" t="s">
         <v>93</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" t="s">
         <v>280</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="E107" t="s">
         <v>281</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G107" s="1" t="s">
+      <c r="F107" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B108" s="1" t="s">
+      <c r="A108" t="s">
+        <v>91</v>
+      </c>
+      <c r="B108" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" t="s">
         <v>188</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" t="s">
         <v>280</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E108" t="s">
         <v>281</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G108" s="1" t="s">
+      <c r="F108" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B109" s="1" t="s">
+      <c r="A109" t="s">
+        <v>91</v>
+      </c>
+      <c r="B109" t="s">
         <v>97</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" t="s">
         <v>98</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" t="s">
         <v>280</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E109" t="s">
         <v>281</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G109" s="1" t="s">
+      <c r="F109" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B110" s="1" t="s">
+      <c r="A110" t="s">
+        <v>91</v>
+      </c>
+      <c r="B110" t="s">
         <v>223</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" t="s">
         <v>224</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" t="s">
         <v>280</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="E110" t="s">
         <v>281</v>
       </c>
-      <c r="F110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G110" s="1" t="s">
+      <c r="F110" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B111" s="1" t="s">
+      <c r="A111" t="s">
+        <v>91</v>
+      </c>
+      <c r="B111" t="s">
         <v>134</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" t="s">
         <v>135</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" t="s">
         <v>282</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E111" t="s">
         <v>283</v>
       </c>
-      <c r="F111" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="1" t="s">
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B112" s="1" t="s">
+      <c r="A112" t="s">
+        <v>91</v>
+      </c>
+      <c r="B112" t="s">
         <v>142</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" t="s">
         <v>143</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" t="s">
         <v>282</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="E112" t="s">
         <v>283</v>
       </c>
-      <c r="F112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="1" t="s">
+      <c r="F112" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B113" s="1" t="s">
+      <c r="A113" t="s">
+        <v>91</v>
+      </c>
+      <c r="B113" t="s">
         <v>145</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" t="s">
         <v>146</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" t="s">
         <v>282</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="E113" t="s">
         <v>283</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G113" s="1" t="s">
+      <c r="F113" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B114" s="1" t="s">
+      <c r="A114" t="s">
+        <v>91</v>
+      </c>
+      <c r="B114" t="s">
         <v>147</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" t="s">
         <v>148</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" t="s">
         <v>282</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="E114" t="s">
         <v>283</v>
       </c>
-      <c r="F114" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="1" t="s">
+      <c r="F114" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B115" s="1" t="s">
+      <c r="A115" t="s">
+        <v>91</v>
+      </c>
+      <c r="B115" t="s">
         <v>270</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" t="s">
         <v>271</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" t="s">
         <v>282</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E115" t="s">
         <v>283</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G115" s="1" t="s">
+      <c r="F115" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B116" s="1" t="s">
+      <c r="A116" t="s">
+        <v>91</v>
+      </c>
+      <c r="B116" t="s">
         <v>107</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" t="s">
         <v>108</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" t="s">
         <v>282</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="E116" t="s">
         <v>283</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G116" s="1" t="s">
+      <c r="F116" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B117" s="1" t="s">
+      <c r="A117" t="s">
+        <v>91</v>
+      </c>
+      <c r="B117" t="s">
         <v>92</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" t="s">
         <v>93</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" t="s">
         <v>284</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="E117" t="s">
         <v>285</v>
       </c>
-      <c r="F117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G117" s="1" t="s">
+      <c r="F117" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B118" s="1" t="s">
+      <c r="A118" t="s">
+        <v>91</v>
+      </c>
+      <c r="B118" t="s">
         <v>276</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" t="s">
         <v>277</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" t="s">
         <v>284</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E118" t="s">
         <v>285</v>
       </c>
-      <c r="F118" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G118" s="1" t="s">
+      <c r="F118" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>